<commit_message>
Bug List: Update the documents of the Bug List
sign-off-by: uvptools@huawei.com
</commit_message>
<xml_diff>
--- a/docs/Linux发行版缺陷列表.xlsx
+++ b/docs/Linux发行版缺陷列表.xlsx
@@ -4,18 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="15" windowWidth="17445" windowHeight="10260" activeTab="2"/>
+    <workbookView xWindow="210" yWindow="15" windowWidth="17445" windowHeight="10260"/>
   </bookViews>
   <sheets>
-    <sheet name="封面" sheetId="3" r:id="rId1"/>
-    <sheet name="前言" sheetId="2" r:id="rId2"/>
-    <sheet name="缺陷列表" sheetId="1" r:id="rId3"/>
+    <sheet name="前言" sheetId="2" r:id="rId1"/>
+    <sheet name="缺陷列表" sheetId="1" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">封面!$A$1:$E$24</definedName>
     <definedName name="unitENG">[1]数据固化!$AB$4:$AB$21</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -23,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="137">
   <si>
     <t>官方补丁链接</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -67,161 +65,6 @@
   <si>
     <t>第一次正式发布。</t>
     <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>文档版本</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>01</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>发布日期</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>华为技术有限公司</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>版权所有</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> © </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="黑体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>华为技术有限公司</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 2016</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="黑体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>。</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="黑体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>保留一切权利。</t>
-    </r>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>非经本公司书面许可，任何单位和个人不得擅自摘抄、复制本文档内容的部分或全部，并不得以任何形式传播。</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>商标声明</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     和其他华为商标均为华为技术有限公司的商标。</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>本文档提及的其他所有商标或注册商标，由各自的所有人拥有。</t>
-  </si>
-  <si>
-    <t>注意</t>
-  </si>
-  <si>
-    <t>您购买的产品、服务或特性等应受华为公司商业合同和条款的约束，本文档中描述的全部或部分产品、服务或特性可能不在您的购买或使用范围之内。除非合同另有约定，华为公司对本文档内容不做任何明示或暗示的声明或保证。</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>由于产品版本升级或其他原因，本文档内容会不定期进行更新。除非另有约定，本文档仅作为使用指导，本文档中的所有陈述、信息和建议不构成任何明示或暗示的担保。</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>华为技术有限公司</t>
-  </si>
-  <si>
-    <t>地址：</t>
-  </si>
-  <si>
-    <r>
-      <t>深圳市龙岗区坂田华为总部办公楼</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">     </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>邮编：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>518129</t>
-    </r>
-  </si>
-  <si>
-    <t>网址：</t>
-  </si>
-  <si>
-    <t>http://www.huawei.com</t>
-  </si>
-  <si>
-    <t>客户服务邮箱：</t>
-  </si>
-  <si>
-    <t>support@huawei.com</t>
-  </si>
-  <si>
-    <t>客户服务电话：</t>
   </si>
   <si>
     <t>序号</t>
@@ -3054,10 +2897,6 @@
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>Linux发行版缺陷列表</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
     <t>本文档给出Linux发行版的缺陷列表。</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
@@ -5350,11 +5189,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5491,85 +5329,10 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color indexed="12"/>
-      <name val="黑体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="12"/>
-      <name val="黑体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.5"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="黑体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="黑体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <name val="黑体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -5578,26 +5341,6 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10.5"/>
@@ -5722,22 +5465,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5804,104 +5544,14 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="35" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5922,11 +5572,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
-    <cellStyle name="常规_sheet" xfId="2"/>
-    <cellStyle name="超链接 2" xfId="3"/>
+    <cellStyle name="超链接 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -5939,149 +5588,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 9" descr="image001.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="904875"/>
-          <a:ext cx="6591300" cy="3286125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>676275</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>990600</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1600200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 93" descr="附件1-16K"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6048375" y="6734175"/>
-          <a:ext cx="942975" cy="923925"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 16" descr="附件3-版权声明页图"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="28575" y="9134475"/>
-          <a:ext cx="295275" cy="285750"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6491,360 +5997,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J38"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="11.25" style="23" customWidth="1"/>
-    <col min="2" max="2" width="13.375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="54.125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="13.375" style="23" customWidth="1"/>
-    <col min="5" max="5" width="11.25" style="23" customWidth="1"/>
-    <col min="6" max="41" width="10.625" style="23" customWidth="1"/>
-    <col min="42" max="16384" width="0" style="23" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="35.1" customHeight="1">
-      <c r="A1" s="22"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="42"/>
-    </row>
-    <row r="2" spans="1:10" ht="37.35" customHeight="1">
-      <c r="A2" s="22"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="42"/>
-    </row>
-    <row r="3" spans="1:10" ht="259.35000000000002" customHeight="1">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="42"/>
-    </row>
-    <row r="4" spans="1:10" ht="111.6" customHeight="1">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="42"/>
-    </row>
-    <row r="5" spans="1:10" ht="18.600000000000001" customHeight="1">
-      <c r="A5" s="44"/>
-      <c r="B5" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="42"/>
-    </row>
-    <row r="6" spans="1:10" ht="18.600000000000001" customHeight="1">
-      <c r="A6" s="44"/>
-      <c r="B6" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="36">
-        <v>42479</v>
-      </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="42"/>
-    </row>
-    <row r="7" spans="1:10" ht="130.35" customHeight="1">
-      <c r="A7" s="44"/>
-      <c r="B7" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="42"/>
-    </row>
-    <row r="8" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A8" s="44"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-    </row>
-    <row r="9" spans="1:10" ht="33" customHeight="1">
-      <c r="A9" s="44"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="42"/>
-      <c r="J9" s="28"/>
-    </row>
-    <row r="10" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A10" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-    </row>
-    <row r="11" spans="1:10" ht="33" customHeight="1">
-      <c r="A11" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="28"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A12" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-    </row>
-    <row r="13" spans="1:10" ht="25.5" customHeight="1">
-      <c r="A13" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-    </row>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A14" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A16" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-    </row>
-    <row r="17" spans="1:10" ht="42" customHeight="1">
-      <c r="A17" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="30"/>
-    </row>
-    <row r="18" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A18" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="30"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75">
-      <c r="A19" s="31"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-    </row>
-    <row r="20" spans="1:10" ht="20.25">
-      <c r="A20" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-    </row>
-    <row r="21" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A21" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-    </row>
-    <row r="22" spans="1:10" ht="20.25" customHeight="1">
-      <c r="A22" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-    </row>
-    <row r="23" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A23" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-    </row>
-    <row r="24" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A24" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="52">
-        <v>4008302118</v>
-      </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-    </row>
-    <row r="36" ht="13.5" customHeight="1"/>
-    <row r="37" ht="13.5" customHeight="1"/>
-    <row r="38" ht="13.5" customHeight="1"/>
-  </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:E9"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-  </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B23" r:id="rId1" display="mailto:Support@huawei.com"/>
-    <hyperlink ref="B22:D22" r:id="rId2" display="http://www.huawei.com"/>
-  </hyperlinks>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="1.5748031496062993" bottom="0.15748031496062992" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="96" orientation="portrait" r:id="rId3"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="8" max="4" man="1"/>
-  </rowBreaks>
-  <drawing r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
@@ -6863,10 +6018,10 @@
     </row>
     <row r="2" spans="1:3" ht="72" customHeight="1">
       <c r="A2" s="11"/>
-      <c r="B2" s="59" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="59"/>
+      <c r="B2" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="29"/>
     </row>
     <row r="3" spans="1:3" ht="22.5">
       <c r="A3" s="9" t="s">
@@ -6876,74 +6031,74 @@
     </row>
     <row r="4" spans="1:3" ht="114" customHeight="1">
       <c r="A4" s="11"/>
-      <c r="B4" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="59"/>
+      <c r="B4" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:3" ht="22.5">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="13"/>
     </row>
     <row r="7" spans="1:3" ht="13.5" customHeight="1">
       <c r="A7" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="56"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="26"/>
     </row>
     <row r="8" spans="1:3" ht="13.5" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="56"/>
+        <v>19</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="26"/>
     </row>
     <row r="9" spans="1:3" ht="13.5" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="56"/>
+        <v>17</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="26"/>
     </row>
     <row r="10" spans="1:3" ht="13.5" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="56"/>
+        <v>18</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="26"/>
     </row>
     <row r="11" spans="1:3" ht="13.5" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="56"/>
+      <c r="B11" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="26"/>
     </row>
     <row r="12" spans="1:3" ht="13.5" customHeight="1">
       <c r="A12" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="58"/>
+        <v>12</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:3" ht="13.5" customHeight="1">
       <c r="A13" s="16"/>
@@ -6963,10 +6118,10 @@
     </row>
     <row r="16" spans="1:3" ht="24" customHeight="1">
       <c r="A16" s="11"/>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="55"/>
+      <c r="C16" s="25"/>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1">
       <c r="A17" s="18" t="s">
@@ -7023,11 +6178,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="C20" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -7043,22 +6198,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="27.75" thickBot="1">
@@ -7066,19 +6221,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="81.75" thickBot="1">
@@ -7086,19 +6241,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="53.25" thickBot="1">
@@ -7106,19 +6261,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="65.25" thickBot="1">
@@ -7126,19 +6281,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="27.75" thickBot="1">
@@ -7146,19 +6301,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="122.25" thickBot="1">
@@ -7166,19 +6321,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="189.75" thickBot="1">
@@ -7186,19 +6341,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="132" customHeight="1" thickBot="1">
@@ -7206,19 +6361,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="67.5" thickBot="1">
@@ -7226,19 +6381,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="53.25" thickBot="1">
@@ -7246,19 +6401,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="41.25" thickBot="1">
@@ -7266,19 +6421,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="81.75" thickBot="1">
@@ -7286,19 +6441,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="81.75" thickBot="1">
@@ -7306,19 +6461,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="81.75" thickBot="1">
@@ -7326,19 +6481,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="129.75" customHeight="1" thickBot="1">
@@ -7346,19 +6501,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="95.25" thickBot="1">
@@ -7366,19 +6521,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="40.5" thickBot="1">
@@ -7386,19 +6541,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="90.75" customHeight="1" thickBot="1">
@@ -7406,159 +6561,159 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="95.25" thickBot="1">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>157</v>
+      <c r="B20" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>136</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F20" s="38" t="s">
-        <v>150</v>
+        <v>101</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="27.75" thickBot="1">
-      <c r="A21" s="37">
+      <c r="A21" s="22">
         <v>20</v>
       </c>
-      <c r="B21" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" s="37" t="s">
-        <v>128</v>
+      <c r="B21" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>107</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="54.75" thickBot="1">
-      <c r="A22" s="37">
+      <c r="A22" s="22">
         <v>21</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="D22" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="54.75" thickBot="1">
-      <c r="A23" s="37">
+      <c r="A23" s="22">
         <v>22</v>
       </c>
-      <c r="B23" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="D23" s="37" t="s">
-        <v>136</v>
+      <c r="B23" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>115</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="243.75" thickBot="1">
-      <c r="A24" s="37">
+      <c r="A24" s="22">
         <v>23</v>
       </c>
-      <c r="B24" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="D24" s="39" t="s">
-        <v>140</v>
+      <c r="B24" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>119</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="80.25" thickBot="1">
-      <c r="A25" s="37">
+      <c r="A25" s="22">
         <v>24</v>
       </c>
-      <c r="B25" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="C25" s="37" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" s="39" t="s">
-        <v>142</v>
+      <c r="B25" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>121</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="51.75" thickBot="1">
-      <c r="A26" s="37">
+      <c r="A26" s="22">
         <v>25</v>
       </c>
-      <c r="B26" s="37" t="s">
-        <v>145</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="D26" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="E26" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="F26" s="37" t="s">
-        <v>143</v>
+      <c r="B26" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>